<commit_message>
Move the Simulink Bus objects and script for creation
</commit_message>
<xml_diff>
--- a/src/model/body/Datos Aero DBX v2.xlsx
+++ b/src/model/body/Datos Aero DBX v2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Documents\Estudios y formación academica\Proyectos\xxcopter\trunk\Modelling and Control\DroneBoX\Modelo CFD DroneBoX\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\Estudios y formación academica\Proyectos\DBX Drones\dronebox-fcs\src\model\body\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Estimaciones teóricas" sheetId="3" r:id="rId3"/>
     <sheet name="Raw Data" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -243,7 +243,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="#,##0.0000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
@@ -441,7 +441,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -733,7 +733,7 @@
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="17.85546875" customWidth="1"/>
   </cols>
@@ -3818,7 +3818,7 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.5703125" customWidth="1"/>
   </cols>
@@ -4081,7 +4081,7 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.140625" customWidth="1"/>
   </cols>
@@ -4481,7 +4481,7 @@
       <selection activeCell="K1" sqref="K1:M131"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -5505,7 +5505,7 @@
         <v>1.8894631765860634</v>
       </c>
       <c r="M25">
-        <v>0.185515465244568</v>
+        <v>0.18551546524456805</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
@@ -5833,7 +5833,7 @@
         <v>2.0723566497411938</v>
       </c>
       <c r="M33">
-        <v>0.20889586694965206</v>
+        <v>0.20889586694965218</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
@@ -6120,7 +6120,7 @@
         <v>1.3262807185602445</v>
       </c>
       <c r="M40">
-        <v>0.11229630545204901</v>
+        <v>0.11229630545204904</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
@@ -6284,7 +6284,7 @@
         <v>2.0978593483260881</v>
       </c>
       <c r="M44">
-        <v>0.22781791913729374</v>
+        <v>0.2278179191372938</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
@@ -6571,7 +6571,7 @@
         <v>1.3793364748992825</v>
       </c>
       <c r="M51">
-        <v>0.12839220907583238</v>
+        <v>0.1283922090758324</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.2">
@@ -6735,7 +6735,7 @@
         <v>1.9819318724196169</v>
       </c>
       <c r="M55">
-        <v>0.19358558920892258</v>
+        <v>0.19358558920892263</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.2">
@@ -7022,7 +7022,7 @@
         <v>1.2524332145926234</v>
       </c>
       <c r="M62">
-        <v>0.10312727102546061</v>
+        <v>0.10312727102546064</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.2">
@@ -7186,7 +7186,7 @@
         <v>1.7188310547800971</v>
       </c>
       <c r="M66">
-        <v>0.18057897860079045</v>
+        <v>0.1805789786007905</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.2">
@@ -7637,7 +7637,7 @@
         <v>1.6729920468744219</v>
       </c>
       <c r="M77">
-        <v>0.18973596636879836</v>
+        <v>0.18973596636879841</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.2">
@@ -7924,7 +7924,7 @@
         <v>0.9455182048243409</v>
       </c>
       <c r="M84">
-        <v>0.11136843282871728</v>
+        <v>0.11136843282871729</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.2">
@@ -8088,7 +8088,7 @@
         <v>1.8022656147480305</v>
       </c>
       <c r="M88">
-        <v>0.18040081579186187</v>
+        <v>0.18040081579186193</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.2">
@@ -8375,7 +8375,7 @@
         <v>1.0575453182325425</v>
       </c>
       <c r="M95">
-        <v>9.5041918181231075E-2</v>
+        <v>9.5041918181231089E-2</v>
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.2">
@@ -8539,7 +8539,7 @@
         <v>1.8127020062726227</v>
       </c>
       <c r="M99">
-        <v>0.1777627280397478</v>
+        <v>0.17776272803974785</v>
       </c>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.2">
@@ -8662,7 +8662,7 @@
         <v>0.72020938901401477</v>
       </c>
       <c r="M102">
-        <v>5.6903913815647508E-2</v>
+        <v>5.6903913815647522E-2</v>
       </c>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.2">
@@ -8703,7 +8703,7 @@
         <v>1.0692906279386272</v>
       </c>
       <c r="M103">
-        <v>8.7429243252462749E-2</v>
+        <v>8.7429243252462763E-2</v>
       </c>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.2">
@@ -8782,7 +8782,7 @@
         <v>6.5520842415802702E-3</v>
       </c>
       <c r="L105">
-        <v>6.71442265757278E-2</v>
+        <v>6.7144226575727814E-2</v>
       </c>
       <c r="M105">
         <v>6.7279658631792763E-2</v>
@@ -8867,7 +8867,7 @@
         <v>1.6047705833257557</v>
       </c>
       <c r="M107">
-        <v>0.20035054592369858</v>
+        <v>0.20035054592369864</v>
       </c>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.2">
@@ -9031,7 +9031,7 @@
         <v>0.90884784585525014</v>
       </c>
       <c r="M111">
-        <v>0.1118406496414306</v>
+        <v>0.11184064964143062</v>
       </c>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.2">
@@ -9523,7 +9523,7 @@
         <v>1.8604870559400697</v>
       </c>
       <c r="M123">
-        <v>0.18121187790161089</v>
+        <v>0.18121187790161095</v>
       </c>
     </row>
     <row r="124" spans="1:13" x14ac:dyDescent="0.2">
@@ -9646,7 +9646,7 @@
         <v>0.77115217116192813</v>
       </c>
       <c r="M126">
-        <v>5.6781453340377042E-2</v>
+        <v>5.6781453340377055E-2</v>
       </c>
     </row>
     <row r="127" spans="1:13" x14ac:dyDescent="0.2">
@@ -9687,7 +9687,7 @@
         <v>1.1261908593889041</v>
       </c>
       <c r="M127">
-        <v>9.1215745471783752E-2</v>
+        <v>9.121574547178378E-2</v>
       </c>
     </row>
     <row r="128" spans="1:13" x14ac:dyDescent="0.2">
@@ -9769,7 +9769,7 @@
         <v>0.12197104710511522</v>
       </c>
       <c r="M129">
-        <v>6.3759664211753816E-2</v>
+        <v>6.3759664211753803E-2</v>
       </c>
     </row>
     <row r="130" spans="1:13" x14ac:dyDescent="0.2">

</xml_diff>